<commit_message>
Atualizado Categorias para os PAD (LIcitação, Dispensa ou Registro de Preços
</commit_message>
<xml_diff>
--- a/Mapeamento lote 02.xlsx
+++ b/Mapeamento lote 02.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="9280.2016" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="544">
   <si>
     <t>1ª) 086ZE  </t>
   </si>
@@ -1755,6 +1755,18 @@
   </si>
   <si>
     <t>Contratação de serviços de manutenção predial para os prédios de Curitiba e interior do Estado -PGE INCORPORADORA DE OBRAS LTDA - ME - Contrato 17/2013.</t>
+  </si>
+  <si>
+    <t>DADOS EXTRAIDOS:</t>
+  </si>
+  <si>
+    <t>DADOS AGRUPADOS:</t>
+  </si>
+  <si>
+    <t>DEPTO</t>
+  </si>
+  <si>
+    <t>NR DIAS</t>
   </si>
 </sst>
 </file>
@@ -1964,7 +1976,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2022,6 +2034,20 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2034,17 +2060,11 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11370,13 +11390,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -11410,13 +11430,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -11450,13 +11470,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -13796,8 +13816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13806,13 +13826,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -13825,12 +13845,12 @@
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -13842,13 +13862,13 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -13861,12 +13881,12 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -13878,11 +13898,11 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="4"/>
       <c r="E9" s="1"/>
     </row>
@@ -13896,36 +13916,36 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
@@ -14262,24 +14282,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -14291,13 +14311,13 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -14310,12 +14330,12 @@
     </row>
     <row r="6" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -14327,11 +14347,11 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="4"/>
       <c r="E8" s="1"/>
     </row>
@@ -14345,36 +14365,36 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -14983,24 +15003,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -15012,13 +15032,13 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -15031,12 +15051,12 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -15048,13 +15068,13 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -15066,11 +15086,11 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
     </row>
@@ -15093,27 +15113,27 @@
       <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
@@ -15809,12 +15829,12 @@
       <c r="A1" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -15826,13 +15846,13 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="31" t="s">
         <v>538</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -15845,12 +15865,12 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="32" t="s">
         <v>286</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -15862,11 +15882,11 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="4"/>
       <c r="E7" s="1"/>
     </row>
@@ -15880,36 +15900,36 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
@@ -16704,10 +16724,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C67"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16715,171 +16735,197 @@
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>537</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="2" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
         <v>539</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="4"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="32" t="s">
         <v>409</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="4"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
         <v>410</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-    </row>
-    <row r="11" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+    </row>
+    <row r="11" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>170</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
         <v>411</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-    </row>
-    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+    </row>
+    <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>172</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="45" t="s">
         <v>412</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
         <v>413</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="9"/>
+      <c r="F18" s="8"/>
+      <c r="I18" s="24" t="s">
+        <v>540</v>
+      </c>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="24" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>68</v>
       </c>
@@ -16892,11 +16938,19 @@
       <c r="D19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="10"/>
+      <c r="F19" s="10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I19" s="24" t="s">
+        <v>542</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>543</v>
+      </c>
+      <c r="M19" s="25"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>414</v>
       </c>
@@ -16909,11 +16963,15 @@
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="23">
+        <f t="shared" ref="E20:E67" si="0">VALUE(IF(LEFT(D20,1)="&lt;",1,LEFT(D20,2)))</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>177</v>
       </c>
@@ -16926,11 +16984,15 @@
       <c r="D21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="14" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>418</v>
       </c>
@@ -16943,11 +17005,15 @@
       <c r="D22" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="E22" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>421</v>
       </c>
@@ -16960,11 +17026,15 @@
       <c r="D23" s="14" t="s">
         <v>423</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="23">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F23" s="14" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="52.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>186</v>
       </c>
@@ -16977,11 +17047,15 @@
       <c r="D24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E24" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>300</v>
       </c>
@@ -16994,11 +17068,15 @@
       <c r="D25" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F25" s="14" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>303</v>
       </c>
@@ -17011,11 +17089,15 @@
       <c r="D26" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="23">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>307</v>
       </c>
@@ -17028,11 +17110,15 @@
       <c r="D27" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F27" s="14" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>29</v>
       </c>
@@ -17045,11 +17131,15 @@
       <c r="D28" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>435</v>
       </c>
@@ -17062,11 +17152,15 @@
       <c r="D29" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="14" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>438</v>
       </c>
@@ -17079,11 +17173,15 @@
       <c r="D30" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>441</v>
       </c>
@@ -17096,11 +17194,15 @@
       <c r="D31" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="14" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>43</v>
       </c>
@@ -17113,11 +17215,15 @@
       <c r="D32" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>211</v>
       </c>
@@ -17130,11 +17236,15 @@
       <c r="D33" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F33" s="14" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>214</v>
       </c>
@@ -17147,11 +17257,15 @@
       <c r="D34" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="12" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>217</v>
       </c>
@@ -17164,11 +17278,15 @@
       <c r="D35" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F35" s="14" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>452</v>
       </c>
@@ -17181,11 +17299,15 @@
       <c r="D36" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F36" s="12" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>223</v>
       </c>
@@ -17198,11 +17320,15 @@
       <c r="D37" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F37" s="14" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>226</v>
       </c>
@@ -17215,11 +17341,15 @@
       <c r="D38" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F38" s="12" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>457</v>
       </c>
@@ -17232,11 +17362,15 @@
       <c r="D39" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F39" s="14" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>459</v>
       </c>
@@ -17249,11 +17383,15 @@
       <c r="D40" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F40" s="12" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>462</v>
       </c>
@@ -17266,11 +17404,15 @@
       <c r="D41" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F41" s="14" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>465</v>
       </c>
@@ -17283,11 +17425,15 @@
       <c r="D42" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F42" s="12" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>240</v>
       </c>
@@ -17300,11 +17446,15 @@
       <c r="D43" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F43" s="14" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>243</v>
       </c>
@@ -17317,11 +17467,15 @@
       <c r="D44" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F44" s="12" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>471</v>
       </c>
@@ -17334,11 +17488,15 @@
       <c r="D45" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F45" s="14" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>474</v>
       </c>
@@ -17351,11 +17509,15 @@
       <c r="D46" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F46" s="12" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>361</v>
       </c>
@@ -17368,11 +17530,15 @@
       <c r="D47" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F47" s="14" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>479</v>
       </c>
@@ -17385,11 +17551,15 @@
       <c r="D48" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F48" s="12" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>482</v>
       </c>
@@ -17402,11 +17572,15 @@
       <c r="D49" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="E49" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F49" s="14" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>485</v>
       </c>
@@ -17419,11 +17593,15 @@
       <c r="D50" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="E50" s="12" t="s">
+      <c r="E50" s="23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="F50" s="12" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>489</v>
       </c>
@@ -17436,11 +17614,15 @@
       <c r="D51" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F51" s="14" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>267</v>
       </c>
@@ -17453,11 +17635,15 @@
       <c r="D52" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="12" t="s">
+      <c r="E52" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F52" s="12" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>270</v>
       </c>
@@ -17470,11 +17656,15 @@
       <c r="D53" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F53" s="14" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>496</v>
       </c>
@@ -17487,11 +17677,15 @@
       <c r="D54" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="12" t="s">
+      <c r="E54" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F54" s="12" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>498</v>
       </c>
@@ -17504,11 +17698,15 @@
       <c r="D55" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F55" s="14" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>501</v>
       </c>
@@ -17521,11 +17719,15 @@
       <c r="D56" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F56" s="12" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>504</v>
       </c>
@@ -17538,11 +17740,15 @@
       <c r="D57" s="14" t="s">
         <v>506</v>
       </c>
-      <c r="E57" s="14" t="s">
+      <c r="E57" s="23">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F57" s="14" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>508</v>
       </c>
@@ -17555,11 +17761,15 @@
       <c r="D58" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F58" s="12" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>511</v>
       </c>
@@ -17572,11 +17782,15 @@
       <c r="D59" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="E59" s="23">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F59" s="14" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="42" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>514</v>
       </c>
@@ -17589,11 +17803,15 @@
       <c r="D60" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E60" s="12" t="s">
+      <c r="E60" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F60" s="12" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>517</v>
       </c>
@@ -17606,11 +17824,15 @@
       <c r="D61" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" s="23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F61" s="14" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>520</v>
       </c>
@@ -17623,11 +17845,15 @@
       <c r="D62" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="E62" s="12" t="s">
+      <c r="E62" s="23">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="F62" s="12" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>523</v>
       </c>
@@ -17640,11 +17866,15 @@
       <c r="D63" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E63" s="14" t="s">
+      <c r="E63" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F63" s="14" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>526</v>
       </c>
@@ -17657,11 +17887,15 @@
       <c r="D64" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E64" s="12" t="s">
+      <c r="E64" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F64" s="12" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>529</v>
       </c>
@@ -17674,11 +17908,15 @@
       <c r="D65" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F65" s="14" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>532</v>
       </c>
@@ -17691,11 +17929,15 @@
       <c r="D66" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E66" s="12" t="s">
+      <c r="E66" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F66" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>534</v>
       </c>
@@ -17708,24 +17950,38 @@
       <c r="D67" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E67" s="14" t="s">
+      <c r="E67" s="23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F67" s="14" t="s">
         <v>536</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A10:F10"/>
   </mergeCells>
+  <conditionalFormatting sqref="E20:E67">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" tooltip="Ver processo" display="http://pad.tre-pr.gov.br/pad/processo/ver_processo.jsp?vp=PROCESSO_LOCALIZAR&amp;tr=1379518810945431&amp;ev=1379518917008252"/>
   </hyperlinks>

</xml_diff>

<commit_message>
dicionado mais PAD para o consolidador
</commit_message>
<xml_diff>
--- a/Mapeamento lote 02.xlsx
+++ b/Mapeamento lote 02.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="9280.2016" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="PAD. 785.2016" sheetId="4" r:id="rId4"/>
     <sheet name="PAD 8354.2012" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -221,9 +221,6 @@
     <t>Assunto</t>
   </si>
   <si>
-    <t xml:space="preserve">Instalação de película na CAE. </t>
-  </si>
-  <si>
     <t>Classificação</t>
   </si>
   <si>
@@ -1767,6 +1764,9 @@
   </si>
   <si>
     <t>NR DIAS</t>
+  </si>
+  <si>
+    <t>Instalação de película na CAE.</t>
   </si>
 </sst>
 </file>
@@ -2093,15 +2093,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2110,6 +2110,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -13528,9 +13531,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -13568,9 +13571,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -13605,7 +13608,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -13640,7 +13643,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -13816,8 +13819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13827,7 +13830,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -13863,7 +13866,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>59</v>
+        <v>543</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -13872,7 +13875,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -13882,7 +13885,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="32"/>
@@ -13890,7 +13893,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -13899,7 +13902,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
@@ -13908,7 +13911,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -13917,7 +13920,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
@@ -13933,7 +13936,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="28"/>
       <c r="C13" s="28"/>
@@ -13950,7 +13953,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
@@ -13958,19 +13961,19 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="C16" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -14268,8 +14271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14283,7 +14286,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -14292,10 +14295,10 @@
     </row>
     <row r="2" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
@@ -14312,7 +14315,7 @@
     </row>
     <row r="4" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -14321,7 +14324,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -14331,7 +14334,7 @@
     <row r="6" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
@@ -14339,7 +14342,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -14348,7 +14351,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
@@ -14357,7 +14360,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -14366,7 +14369,7 @@
     </row>
     <row r="10" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
@@ -14382,7 +14385,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
@@ -14399,7 +14402,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
@@ -14407,30 +14410,30 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="E15" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>3</v>
@@ -14441,16 +14444,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>83</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>11</v>
@@ -14458,30 +14461,30 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>87</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>88</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>3</v>
@@ -14492,53 +14495,53 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>89</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>90</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>41</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>92</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>93</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>95</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>96</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -14546,16 +14549,16 @@
         <v>26</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -14563,10 +14566,10 @@
         <v>29</v>
       </c>
       <c r="B24" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>98</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>99</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>3</v>
@@ -14580,10 +14583,10 @@
         <v>32</v>
       </c>
       <c r="B25" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>99</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>3</v>
@@ -14597,10 +14600,10 @@
         <v>35</v>
       </c>
       <c r="B26" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>100</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>101</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>24</v>
@@ -14611,33 +14614,33 @@
     </row>
     <row r="27" spans="1:5" ht="42" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="E27" s="14" t="s">
         <v>104</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="13" t="s">
+      <c r="D28" s="12" t="s">
         <v>107</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>11</v>
@@ -14645,183 +14648,183 @@
     </row>
     <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>109</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>110</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>112</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>113</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="42" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>116</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>118</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>119</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>121</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>122</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>128</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>131</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="42" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C37" s="15" t="s">
+      <c r="D37" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E37" s="14" t="s">
         <v>134</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>136</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>137</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>139</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>140</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>3</v>
@@ -14832,13 +14835,13 @@
     </row>
     <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>142</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>3</v>
@@ -14849,98 +14852,98 @@
     </row>
     <row r="41" spans="1:5" ht="42" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="C41" s="15" t="s">
+      <c r="D41" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="E41" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="E41" s="14" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="13" t="s">
+      <c r="D42" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="E42" s="12" t="s">
         <v>149</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>151</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>152</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>154</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>155</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>158</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" s="13" t="s">
         <v>160</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>161</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>3</v>
@@ -14951,13 +14954,13 @@
     </row>
     <row r="47" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>162</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>163</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>20</v>
@@ -14989,8 +14992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15004,7 +15007,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -15013,10 +15016,10 @@
     </row>
     <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
@@ -15033,7 +15036,7 @@
     </row>
     <row r="4" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
@@ -15042,7 +15045,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -15052,7 +15055,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
@@ -15060,7 +15063,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -15069,7 +15072,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
@@ -15078,7 +15081,7 @@
     </row>
     <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -15087,7 +15090,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
@@ -15096,7 +15099,7 @@
     </row>
     <row r="11" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -15105,7 +15108,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -15121,7 +15124,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
@@ -15138,7 +15141,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
@@ -15146,30 +15149,30 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>3</v>
@@ -15180,155 +15183,155 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>177</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>178</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>180</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>181</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>183</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>184</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>186</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>187</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>189</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>190</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>192</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>193</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>195</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>196</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>198</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>199</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>201</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>202</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -15336,33 +15339,33 @@
         <v>35</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="42" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>206</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>207</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.25">
@@ -15370,180 +15373,180 @@
         <v>43</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>211</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>212</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>214</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>215</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>217</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>218</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>220</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>221</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>223</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>224</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>226</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>227</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>229</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>230</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>232</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>233</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>236</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>238</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>239</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>3</v>
@@ -15554,132 +15557,132 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>240</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>241</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>243</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>244</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>246</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>247</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>249</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>250</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>252</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>253</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="C46" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="C46" s="13" t="s">
+      <c r="D46" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="E46" s="12" t="s">
         <v>257</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>259</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>260</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>262</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>263</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>3</v>
@@ -15690,104 +15693,104 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="C49" s="15" t="s">
         <v>264</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>265</v>
       </c>
       <c r="D49" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C50" s="13" t="s">
         <v>267</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>268</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>270</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>268</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>271</v>
       </c>
       <c r="D51" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C52" s="13" t="s">
         <v>273</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>274</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="C53" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="B53" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="C53" s="15" t="s">
+      <c r="D53" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="E53" s="14" t="s">
         <v>278</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C54" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="B54" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="C54" s="13" t="s">
+      <c r="D54" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="E54" s="12" t="s">
         <v>282</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -15813,8 +15816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15827,10 +15830,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
@@ -15847,7 +15850,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
@@ -15856,7 +15859,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -15866,7 +15869,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
@@ -15874,7 +15877,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -15883,7 +15886,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
@@ -15892,7 +15895,7 @@
     </row>
     <row r="8" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -15901,7 +15904,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
@@ -15917,7 +15920,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -15934,7 +15937,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
@@ -15942,30 +15945,30 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>3</v>
@@ -15976,16 +15979,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>291</v>
-      </c>
       <c r="D16" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>11</v>
@@ -15993,472 +15996,472 @@
     </row>
     <row r="17" spans="1:5" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="D17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>293</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C18" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="E18" s="14" t="s">
         <v>296</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>300</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>301</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>305</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>307</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>308</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>310</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>311</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>313</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>314</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>316</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>317</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>318</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>319</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="C27" s="13" t="s">
+      <c r="D27" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>322</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>326</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>324</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>327</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>329</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>330</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="C31" s="13" t="s">
         <v>332</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>330</v>
-      </c>
-      <c r="C31" s="13" t="s">
+      <c r="D31" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>333</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D32" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="C33" s="13" t="s">
+      <c r="D33" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>338</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>340</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>341</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="C35" s="13" t="s">
+      <c r="D35" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="E35" s="12" t="s">
         <v>344</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="C37" s="13" t="s">
         <v>348</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>349</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>351</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>349</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>352</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>354</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>355</v>
       </c>
       <c r="D39" s="12" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="42" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="C41" s="13" t="s">
         <v>358</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>359</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="C42" s="15" t="s">
         <v>361</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>359</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>362</v>
       </c>
       <c r="D42" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="C43" s="13" t="s">
         <v>364</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>365</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B44" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>365</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>366</v>
       </c>
       <c r="D44" s="14" t="s">
         <v>3</v>
@@ -16469,98 +16472,98 @@
     </row>
     <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="C45" s="13" t="s">
         <v>367</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>368</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="C46" s="15" t="s">
         <v>370</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>368</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>371</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C47" s="13" t="s">
         <v>373</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>374</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C48" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="D48" s="14" t="s">
         <v>376</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="E48" s="14" t="s">
         <v>377</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>379</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>376</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>380</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>382</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>383</v>
       </c>
       <c r="D50" s="14" t="s">
         <v>3</v>
@@ -16571,47 +16574,47 @@
     </row>
     <row r="51" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>384</v>
       </c>
-      <c r="B51" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="C51" s="13" t="s">
+      <c r="D51" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="12" t="s">
         <v>385</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="C52" s="15" t="s">
         <v>387</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>385</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>388</v>
       </c>
       <c r="D52" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="C53" s="13" t="s">
         <v>390</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>388</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>391</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>3</v>
@@ -16622,87 +16625,87 @@
     </row>
     <row r="54" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
+        <v>391</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="C54" s="15" t="s">
         <v>392</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>391</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>393</v>
       </c>
       <c r="D54" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C55" s="13" t="s">
         <v>395</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>396</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>41</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="C56" s="15" t="s">
         <v>398</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>396</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>399</v>
       </c>
       <c r="D56" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>401</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>399</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>402</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="C58" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="B58" s="15" t="s">
-        <v>402</v>
-      </c>
-      <c r="C58" s="15" t="s">
+      <c r="D58" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="E58" s="14" t="s">
         <v>406</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -16726,8 +16729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16741,7 +16744,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -16751,10 +16754,10 @@
     </row>
     <row r="2" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C2" s="34"/>
       <c r="D2" s="34"/>
@@ -16773,7 +16776,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -16783,7 +16786,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -16794,7 +16797,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="32" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
@@ -16803,7 +16806,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -16813,7 +16816,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
@@ -16823,7 +16826,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -16832,18 +16835,18 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
-        <v>410</v>
-      </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="A10" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
     </row>
     <row r="11" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -16852,18 +16855,18 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
-        <v>411</v>
-      </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
+      <c r="A12" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
     </row>
     <row r="13" spans="1:6" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -16872,11 +16875,11 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
-        <v>412</v>
-      </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
+      <c r="A14" s="44" t="s">
+        <v>411</v>
+      </c>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="1"/>
@@ -16891,7 +16894,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>
@@ -16910,55 +16913,55 @@
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="8"/>
       <c r="I18" s="24" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
       <c r="L18" s="24" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>71</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I19" s="24" t="s">
+        <v>541</v>
+      </c>
+      <c r="J19" s="24" t="s">
         <v>542</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>543</v>
       </c>
       <c r="M19" s="25"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>3</v>
@@ -16973,13 +16976,13 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B21" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>415</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>416</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>20</v>
@@ -16989,18 +16992,18 @@
         <v>1</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>418</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>416</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>419</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>20</v>
@@ -17010,39 +17013,39 @@
         <v>1</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="B23" s="15" t="s">
-        <v>419</v>
-      </c>
-      <c r="C23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>422</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>423</v>
       </c>
       <c r="E23" s="23">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>20</v>
@@ -17052,18 +17055,18 @@
         <v>1</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>41</v>
@@ -17073,39 +17076,39 @@
         <v>5</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E26" s="23">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>3</v>
@@ -17115,7 +17118,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
@@ -17123,10 +17126,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>3</v>
@@ -17136,18 +17139,18 @@
         <v>1</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>435</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>433</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>436</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>20</v>
@@ -17157,18 +17160,18 @@
         <v>1</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>435</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>438</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>436</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>439</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>3</v>
@@ -17178,18 +17181,18 @@
         <v>1</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>438</v>
+      </c>
+      <c r="C31" s="15" t="s">
         <v>441</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>439</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>442</v>
       </c>
       <c r="D31" s="14" t="s">
         <v>3</v>
@@ -17199,7 +17202,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -17207,10 +17210,10 @@
         <v>43</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>37</v>
@@ -17220,18 +17223,18 @@
         <v>2</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>10</v>
@@ -17241,18 +17244,18 @@
         <v>3</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>3</v>
@@ -17262,18 +17265,18 @@
         <v>1</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>37</v>
@@ -17283,18 +17286,18 @@
         <v>2</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
+        <v>451</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>452</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>450</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>453</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>20</v>
@@ -17304,18 +17307,18 @@
         <v>1</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>37</v>
@@ -17325,18 +17328,18 @@
         <v>2</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B38" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="C38" s="13" t="s">
         <v>455</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>456</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>3</v>
@@ -17346,18 +17349,18 @@
         <v>1</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
+        <v>456</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>455</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>457</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>456</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>458</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>3</v>
@@ -17367,18 +17370,18 @@
         <v>1</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
+        <v>458</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>457</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>459</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>458</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>460</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>3</v>
@@ -17388,18 +17391,18 @@
         <v>1</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>459</v>
+      </c>
+      <c r="C41" s="15" t="s">
         <v>462</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>460</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>463</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>3</v>
@@ -17409,18 +17412,18 @@
         <v>1</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
+        <v>464</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>465</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>463</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>466</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>3</v>
@@ -17430,18 +17433,18 @@
         <v>1</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D43" s="14" t="s">
         <v>37</v>
@@ -17451,39 +17454,39 @@
         <v>2</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B44" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>468</v>
       </c>
-      <c r="C44" s="13" t="s">
-        <v>469</v>
-      </c>
       <c r="D44" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E44" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="C45" s="15" t="s">
         <v>471</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>469</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>472</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>3</v>
@@ -17493,18 +17496,18 @@
         <v>1</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="C46" s="13" t="s">
         <v>474</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>472</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>475</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>3</v>
@@ -17514,18 +17517,18 @@
         <v>1</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D47" s="14" t="s">
         <v>24</v>
@@ -17535,18 +17538,18 @@
         <v>4</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
+        <v>478</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>479</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>477</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>480</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>3</v>
@@ -17556,18 +17559,18 @@
         <v>1</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
+        <v>481</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="C49" s="15" t="s">
         <v>482</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>480</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>483</v>
       </c>
       <c r="D49" s="14" t="s">
         <v>3</v>
@@ -17577,39 +17580,39 @@
         <v>1</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="C50" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>483</v>
-      </c>
-      <c r="C50" s="13" t="s">
+      <c r="D50" s="12" t="s">
         <v>486</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>487</v>
       </c>
       <c r="E50" s="23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>485</v>
+      </c>
+      <c r="C51" s="15" t="s">
         <v>489</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>486</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>490</v>
       </c>
       <c r="D51" s="14" t="s">
         <v>3</v>
@@ -17619,18 +17622,18 @@
         <v>1</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>3</v>
@@ -17640,18 +17643,18 @@
         <v>1</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>10</v>
@@ -17661,18 +17664,18 @@
         <v>3</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
+        <v>495</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>493</v>
+      </c>
+      <c r="C54" s="13" t="s">
         <v>496</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>494</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>497</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>3</v>
@@ -17682,18 +17685,18 @@
         <v>1</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
+        <v>497</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="C55" s="15" t="s">
         <v>498</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>497</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>499</v>
       </c>
       <c r="D55" s="14" t="s">
         <v>3</v>
@@ -17703,18 +17706,18 @@
         <v>1</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="C56" s="13" t="s">
         <v>501</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>499</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>502</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>3</v>
@@ -17724,39 +17727,39 @@
         <v>1</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="C57" s="15" t="s">
         <v>504</v>
       </c>
-      <c r="B57" s="15" t="s">
-        <v>502</v>
-      </c>
-      <c r="C57" s="15" t="s">
+      <c r="D57" s="14" t="s">
         <v>505</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>506</v>
       </c>
       <c r="E57" s="23">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>504</v>
+      </c>
+      <c r="C58" s="13" t="s">
         <v>508</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>505</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>509</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>3</v>
@@ -17766,18 +17769,18 @@
         <v>1</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>508</v>
+      </c>
+      <c r="C59" s="15" t="s">
         <v>511</v>
-      </c>
-      <c r="B59" s="15" t="s">
-        <v>509</v>
-      </c>
-      <c r="C59" s="15" t="s">
-        <v>512</v>
       </c>
       <c r="D59" s="14" t="s">
         <v>37</v>
@@ -17787,18 +17790,18 @@
         <v>2</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="42" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>511</v>
+      </c>
+      <c r="C60" s="13" t="s">
         <v>514</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>512</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>515</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>3</v>
@@ -17808,18 +17811,18 @@
         <v>1</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>514</v>
+      </c>
+      <c r="C61" s="15" t="s">
         <v>517</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>515</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>518</v>
       </c>
       <c r="D61" s="14" t="s">
         <v>24</v>
@@ -17829,39 +17832,39 @@
         <v>4</v>
       </c>
       <c r="F61" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
+        <v>519</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>517</v>
+      </c>
+      <c r="C62" s="13" t="s">
         <v>520</v>
       </c>
-      <c r="B62" s="13" t="s">
-        <v>518</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>521</v>
-      </c>
       <c r="D62" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E62" s="23">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>520</v>
+      </c>
+      <c r="C63" s="15" t="s">
         <v>523</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>521</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>524</v>
       </c>
       <c r="D63" s="14" t="s">
         <v>3</v>
@@ -17871,18 +17874,18 @@
         <v>1</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>523</v>
+      </c>
+      <c r="C64" s="13" t="s">
         <v>526</v>
-      </c>
-      <c r="B64" s="13" t="s">
-        <v>524</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>527</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>3</v>
@@ -17892,18 +17895,18 @@
         <v>1</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>526</v>
+      </c>
+      <c r="C65" s="15" t="s">
         <v>529</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>527</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>530</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>3</v>
@@ -17913,18 +17916,18 @@
         <v>1</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>529</v>
+      </c>
+      <c r="C66" s="13" t="s">
         <v>532</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>530</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>533</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>3</v>
@@ -17939,13 +17942,13 @@
     </row>
     <row r="67" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
+        <v>533</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>532</v>
+      </c>
+      <c r="C67" s="15" t="s">
         <v>534</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>533</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>535</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>3</v>
@@ -17955,22 +17958,22 @@
         <v>1</v>
       </c>
       <c r="F67" s="14" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A10:F10"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A10:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="E20:E67">
     <cfRule type="colorScale" priority="1">

</xml_diff>